<commit_message>
Guia definitiva, aumento version
</commit_message>
<xml_diff>
--- a/StructureDefinition-BundleHackaton.xlsx
+++ b/StructureDefinition-BundleHackaton.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-24T10:24:09-04:00</t>
+    <t>2023-07-24T11:34:17-04:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>